<commit_message>
Add date input field to daily supply input page and update data handling for date
</commit_message>
<xml_diff>
--- a/public/excelTemplates/Nhap_Chay_Lo.xlsx
+++ b/public/excelTemplates/Nhap_Chay_Lo.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\DQ_Admin_Panel_Project\DQ_Admin_Panel\public\excelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45773153-F285-4915-97ED-8DBB0E8E09DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D486CF-CF91-428C-853E-2A1774490A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{56748950-8610-46D1-8F15-23048271DE89}"/>
   </bookViews>
   <sheets>
     <sheet name="Bảng nhập" sheetId="1" r:id="rId1"/>
+    <sheet name="Mẫu nhập và lưu ý" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Ngày</t>
   </si>
@@ -51,13 +52,46 @@
   </si>
   <si>
     <t>Thành phẩm</t>
+  </si>
+  <si>
+    <t>34,4</t>
+  </si>
+  <si>
+    <t>34,5</t>
+  </si>
+  <si>
+    <t>Lưu ý chung</t>
+  </si>
+  <si>
+    <t>32,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chỉ nhập các dữ liệu bên trong bảng! </t>
+  </si>
+  <si>
+    <t>Bắt buộc các trường</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Format: dd/mm/yyyy. Khi nhập ngày 0-/0-/yyyy, có thể nó sẽ lược bỏ số 0. Không có vấn đề, giữ nguyên!</t>
+  </si>
+  <si>
+    <t>Không được số âm</t>
+  </si>
+  <si>
+    <t>0 &gt; x &lt; 100. Đơn vị thập phân (Ví dụ: 32,43)</t>
+  </si>
+  <si>
+    <t>Số lượng thành phẩm</t>
+  </si>
+  <si>
+    <t>Ghi đánh giá hoặc lưu ý</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,13 +130,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB8A7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
@@ -127,38 +187,71 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="14">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -171,11 +264,17 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
@@ -202,6 +301,32 @@
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotTable Style 1">
@@ -224,16 +349,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5C5C7DB8-DA59-491A-AD0C-C3E8A1BC6C91}" name="Table2" displayName="Table2" ref="A1:E888" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5C5C7DB8-DA59-491A-AD0C-C3E8A1BC6C91}" name="Table2" displayName="Table2" ref="A1:E888" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:E888" xr:uid="{5C5C7DB8-DA59-491A-AD0C-C3E8A1BC6C91}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{87EBFF84-8493-4D82-8FB8-8D5881FE0EFE}" name="Ngày" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{AECB8577-328B-4830-B036-24C70D649B7B}" name="Số lượng mủ nước" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{62D3B52D-E70C-48A4-8464-27B2788FD59A}" name="Hàm lượng mủ nước" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{A659011C-D5FF-453B-8EF1-ED2274F09682}" name="Thành phẩm" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{4B5565F4-048A-45CB-918D-614ED8DA3CB8}" name="Ghi chú" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{87EBFF84-8493-4D82-8FB8-8D5881FE0EFE}" name="Ngày" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{AECB8577-328B-4830-B036-24C70D649B7B}" name="Số lượng mủ nước" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{62D3B52D-E70C-48A4-8464-27B2788FD59A}" name="Hàm lượng mủ nước" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{A659011C-D5FF-453B-8EF1-ED2274F09682}" name="Thành phẩm" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{4B5565F4-048A-45CB-918D-614ED8DA3CB8}" name="Ghi chú" dataDxfId="7"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{967571E2-DBFB-433D-BB5B-82E093988B7D}" name="Table22" displayName="Table22" ref="A1:E888" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E888" xr:uid="{967571E2-DBFB-433D-BB5B-82E093988B7D}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{1234F11E-8FEA-4628-B892-1FD51FDC432C}" name="Ngày" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{848120E2-6040-4BC0-B3A4-93185E5006D4}" name="Số lượng mủ nước" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{B0A42711-998B-4176-9A67-F74E3ABD851D}" name="Hàm lượng mủ nước" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{874D83DA-D7E3-4B05-BFFD-7E5C02B2F177}" name="Thành phẩm" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{8BEC1EDB-EA09-4702-B45B-A03D8166EBB1}" name="Ghi chú" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -557,7 +696,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +708,7 @@
     <col min="5" max="5" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="93.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="93.140625" style="1" bestFit="1" customWidth="1"/>
@@ -578,79 +717,284 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G6" s="4"/>
-      <c r="H6" s="5"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G7" s="4"/>
-      <c r="H7" s="5"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G8" s="4"/>
-      <c r="H8" s="5"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G9" s="4"/>
-      <c r="H9" s="5"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G10" s="4"/>
-      <c r="H10" s="5"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G11" s="4"/>
-      <c r="H11" s="5"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="Y7zd2FdLFszN/o3wfL2KSgf01NkCV6QRX94F1mwvVgUL1gkTs3CsVFIGx9vwxbp3SSeXMJp4+69JCX+irY/kDQ==" saltValue="ZUEyxarKPBT7CWKqU3joxw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" sort="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED4523D-71B6-460B-8868-2A0A7FEC5D04}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" activeCellId="1" sqref="D12 H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="93.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="5"/>
+    <col min="10" max="10" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="93.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>45658</v>
+      </c>
+      <c r="B2" s="5">
+        <v>87</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>45659</v>
+      </c>
+      <c r="B3" s="5">
+        <v>90</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5">
+        <v>32</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>45660</v>
+      </c>
+      <c r="B4" s="5">
+        <v>78</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5">
+        <v>43</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="9"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="19" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H19" s="3"/>
+      <c r="H19" s="14"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="yQ1+DwscHvnBxZQ2AFbE9RYqvlp4YIsucWK46EQjUAvDNWbRCl/tTc/Hd6j2JqcENcmpTDJ0LM+2xsmw3kzBHA==" saltValue="1r/ntKyJTiA11vzsIy2ifw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="8AZ0TyWIVaTvuZuZszVuXU/pHqiEFgFJ6D2Szah+Q87bmcvw0V+iyYYwiiyI7HxckwmM5MquAwCuTgm2ofl6+g==" saltValue="psG7BgnCkbKxTZ8G5OR0bw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="3">
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>